<commit_message>
nuevos cambios en el readme
</commit_message>
<xml_diff>
--- a/export/clientes_limpios.xlsx
+++ b/export/clientes_limpios.xlsx
@@ -504,7 +504,9 @@
       <c r="B4" t="n">
         <v>10000</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>45122</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Female</t>

</xml_diff>